<commit_message>
Fix: asegurar nombre correcto Login.js para Vercel
</commit_message>
<xml_diff>
--- a/backend/file.xlsx
+++ b/backend/file.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\mi-app-llantas\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A6228CA-E62D-4EED-9712-BA261031821A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C2F1F432-3092-4D99-A54E-5347B52BFD0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14190" yWindow="0" windowWidth="14610" windowHeight="15480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -96,7 +96,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -104,29 +104,17 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -435,17 +423,17 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -469,62 +457,62 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="2">
         <v>220000</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="2">
         <v>280000</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="2">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="2">
         <v>180000</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="2">
         <v>230000</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="2">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="2">
         <v>200000</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="2">
         <v>260000</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="2">
         <v>8</v>
       </c>
     </row>

</xml_diff>